<commit_message>
Commento menu in ApplicazioneTest. DocAggiornata. MappeConEventoMenu
</commit_message>
<xml_diff>
--- a/MappaGenerica.xlsx
+++ b/MappaGenerica.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\UninaCampus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikel_000\Desktop\ProgettoIS2\UninaCampus\UninaCampus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
   <si>
     <t>Azione</t>
   </si>
@@ -902,19 +902,6 @@
     <t>Click su item menu</t>
   </si>
   <si>
-    <r>
-      <t>solo.clickOnMenuItem(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>"ItemMenu1");</t>
-    </r>
-  </si>
-  <si>
     <t>ViewInteraction appCompatImageButton = onView(
                 allOf(withContentDescription("content_description"),
                         childAtPosition(
@@ -927,15 +914,24 @@
         appCompatImageButton.perform(click());</t>
   </si>
   <si>
-    <t>ViewInteraction navigationMenuItemView = onView(
-                allOf(childAtPosition(
-                        allOf(withId(R.id.id_design_navigation_view),
+    <t xml:space="preserve"> openActionBarOverflowOrOptionsMenu(getInstrumentation().getTargetContext());
+        ViewInteraction textView2 = onView(
+                allOf(withId(android.R.id.testo), withText("TestoDaSelezionare"),
+                        childAtPosition(
                                 childAtPosition(
-                                        withId(R.id.id_nvView),
-                                        0)),
-                        1),
-                        isDisplayed()));
-        navigationMenuItemView.perform(click());</t>
+ withClassName(is("com.android.internal.view.menu.ListMenuItemView")),
+                                        PosizioneElemento),
+                                Posizione),
+                        isDisplayed()));
+        textView2.perform(click());</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        shadowOf(activity).clickMenuItem(R.id.ElementoDelMenuDaSelezionare);</t>
+  </si>
+  <si>
+    <t>solo.sendKey(solo.MENU);
+    // Click on Change Settings 
+  solo.clickInList(PosizioneNelMenuDaSelezionare, 0);</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1026,6 +1022,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1411,13 +1410,13 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="D29" sqref="A29:D29"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.7109375" customWidth="1"/>
-    <col min="2" max="2" width="74.140625" customWidth="1"/>
+    <col min="2" max="2" width="77.28515625" customWidth="1"/>
     <col min="3" max="3" width="186.140625" customWidth="1"/>
     <col min="4" max="4" width="139.28515625" customWidth="1"/>
   </cols>
@@ -1805,7 +1804,7 @@
         <v>93</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
         <v>24</v>
@@ -1814,18 +1813,18 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
         <v>98</v>
       </c>
-      <c r="C29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>96</v>
+      <c r="D29" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
copertur di munchlife, di applicazioneTest, paragrafo traduttore Automa
</commit_message>
<xml_diff>
--- a/MappaGenerica.xlsx
+++ b/MappaGenerica.xlsx
@@ -886,35 +886,22 @@
     <t>Apertura menu laterale</t>
   </si>
   <si>
-    <r>
-      <t>solo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>.clickOnActionBarHomeButton();</t>
-    </r>
-  </si>
-  <si>
     <t>Click su item menu</t>
   </si>
   <si>
-    <t>ViewInteraction appCompatImageButton = onView(
-                allOf(withContentDescription("content_description"),
-                        childAtPosition(
-                                allOf(withId(R.id.idToolbar),
-                                        childAtPosition(
-                                                withClassName(is("android.widget.LinearLayout")),
-                                                0)),
-                                1),
-                        isDisplayed()));
-        appCompatImageButton.perform(click());</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> openActionBarOverflowOrOptionsMenu(getInstrumentation().getTargetContext());
+    <t xml:space="preserve">        shadowOf(activity).clickMenuItem(R.id.ElementoDelMenuDaSelezionare);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solo.sendKey(solo.MENU);
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+  solo.clickInList(PosizioneNelMenuDaSelezionare, 0);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
         ViewInteraction textView2 = onView(
                 allOf(withId(android.R.id.testo), withText("TestoDaSelezionare"),
                         childAtPosition(
@@ -923,22 +910,42 @@
                                         PosizioneElemento),
                                 Posizione),
                         isDisplayed()));
-        textView2.perform(click());</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        shadowOf(activity).clickMenuItem(R.id.ElementoDelMenuDaSelezionare);</t>
-  </si>
-  <si>
-    <t>solo.sendKey(solo.MENU);
-    // Click on Change Settings 
-  solo.clickInList(PosizioneNelMenuDaSelezionare, 0);</t>
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    textView2.perform(click());</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>openActionBarOverflowOrOptionsMenu(getInstrumentation().getTargetContext());</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -986,11 +993,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1012,7 +1014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1021,7 +1023,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1409,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,27 +1805,27 @@
         <v>93</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="D29" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="C29" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>